<commit_message>
Updating collaboration.R with 2022 data
</commit_message>
<xml_diff>
--- a/citations/published_brill.xlsx
+++ b/citations/published_brill.xlsx
@@ -685,37 +685,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4388460035</t>
+          <t>https://openalex.org/W4313596414</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Consciousness Is Quantum State Reduction Which Creates the Flow of Time</t>
+          <t>Mummy Labels: A Witness to the Use and Processing of Wood in Roman Egypt</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Consciousness Is Quantum State Reduction Which Creates the Flow of Time</t>
+          <t>Mummy Labels: A Witness to the Use and Processing of Wood in Roman Egypt</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Abstract In neuroscience, the flow of time is a conscious experience produced by the brain. But in physics, time is either a process, or a dimension in four-dimensional spacetime geometry. Could all three explanations be correct? The Penrose–Hameroff ‘Orch OR’ theory suggests consciousness is a sequence of discrete, irreversible quantum state reductions occurring at an objective threshold (‘objective reduction’, ‘OR’) a process in fundamental spacetime geometry. These ‘self-collapses’ of the quantum wavefunction are ‘orchestrated’ in microtubules inside brain neurons. Each Orch OR event selects microtubule states which purposefully regulate neuronal functions, and provide sequences of ‘NOW’ moments of conscious experience. Connected to fundamental spacetime geometry by Penrose ‘OR’, consciousness is quantum state reduction, a set of irreversible steps which ‘ratchet forward’ in the fine scale geometry of the universe, creating a flow of time.</t>
+          <t>Abstract Mummy labels are relics found in large quantities in Egypt, often in an excellent state of preservation (like most woods preserved in arid environments). As a result, they are widespread in Roman Egyptian collections of many museums. These labels reflect funerary practices that possess Egyptian and Roman influences and are an important source of historical and archaeological information. These corpora of mummy labels offer several possibilities for investigation. The inscriptions on these labels have been the subject of an international project (Death on the Nile) in which all accessible objects were recorded in a database. However, the potential of these funerary objects extend beyond the inscriptions to the methods of manufacturing and cutting, the choice of species used, and their dendrochronological potential to better define their chronology and possibly their provenance. The study of mummy labels allows us to propose a new typology, some forms of which seem to be limited to certain necropolises. Mummy labels, whether made by the family of the deceased or by specific workshops, show that their realizations vary greatly, ranging from coarse specimens to others with beautiful detailing. They are made from endemic as well as imported species, which are symbolic of long-distance trade, especially for conifer trees, which are well represented. Their dendrochronological potential has also been demonstrated in numerous studies, some of which have allowed the identification of labels from the same tree, supported by inscriptions attesting to the same family relationship.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-01-04</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Timing &amp; Time Perception</t>
+          <t>International Journal of Wood Culture</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4210181418</t>
+          <t>https://openalex.org/S4210185514</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -725,17 +725,17 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2213-445X</t>
+          <t>2772-3186</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/22134468-bja10098</t>
+          <t>https://doi.org/10.1163/27723194-bja10017</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>https://brill.com/downloadpdf/view/journals/time/aop/article-10.1163-22134468-bja10098/article-10.1163-22134468-bja10098.pdf</t>
+          <t>https://brill.com/downloadpdf/journals/ijwc/aop/article-10.1163-27723194-bja10017/article-10.1163-27723194-bja10017.pdf</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -750,22 +750,22 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>192</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>223</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="S3" t="b">
@@ -776,16 +776,16 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>hybrid</t>
+          <t>diamond</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>https://brill.com/downloadpdf/view/journals/time/aop/article-10.1163-22134468-bja10098/article-10.1163-22134468-bja10098.pdf</t>
+          <t>https://brill.com/downloadpdf/journals/ijwc/aop/article-10.1163-27723194-bja10017/article-10.1163-27723194-bja10017.pdf</t>
         </is>
       </c>
       <c r="W3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -800,12 +800,12 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4388460035</t>
+          <t>https://api.openalex.org/works?filter=cites:W4313596414</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/22134468-bja10098</t>
+          <t>https://doi.org/10.1163/27723194-bja10017</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
@@ -823,37 +823,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4313596414</t>
+          <t>https://openalex.org/W4388460035</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mummy Labels: A Witness to the Use and Processing of Wood in Roman Egypt</t>
+          <t>Consciousness Is Quantum State Reduction Which Creates the Flow of Time</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mummy Labels: A Witness to the Use and Processing of Wood in Roman Egypt</t>
+          <t>Consciousness Is Quantum State Reduction Which Creates the Flow of Time</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Abstract Mummy labels are relics found in large quantities in Egypt, often in an excellent state of preservation (like most woods preserved in arid environments). As a result, they are widespread in Roman Egyptian collections of many museums. These labels reflect funerary practices that possess Egyptian and Roman influences and are an important source of historical and archaeological information. These corpora of mummy labels offer several possibilities for investigation. The inscriptions on these labels have been the subject of an international project (Death on the Nile) in which all accessible objects were recorded in a database. However, the potential of these funerary objects extend beyond the inscriptions to the methods of manufacturing and cutting, the choice of species used, and their dendrochronological potential to better define their chronology and possibly their provenance. The study of mummy labels allows us to propose a new typology, some forms of which seem to be limited to certain necropolises. Mummy labels, whether made by the family of the deceased or by specific workshops, show that their realizations vary greatly, ranging from coarse specimens to others with beautiful detailing. They are made from endemic as well as imported species, which are symbolic of long-distance trade, especially for conifer trees, which are well represented. Their dendrochronological potential has also been demonstrated in numerous studies, some of which have allowed the identification of labels from the same tree, supported by inscriptions attesting to the same family relationship.</t>
+          <t>Abstract In neuroscience, the flow of time is a conscious experience produced by the brain. But in physics, time is either a process, or a dimension in four-dimensional spacetime geometry. Could all three explanations be correct? The Penrose–Hameroff ‘Orch OR’ theory suggests consciousness is a sequence of discrete, irreversible quantum state reductions occurring at an objective threshold (‘objective reduction’, ‘OR’) a process in fundamental spacetime geometry. These ‘self-collapses’ of the quantum wavefunction are ‘orchestrated’ in microtubules inside brain neurons. Each Orch OR event selects microtubule states which purposefully regulate neuronal functions, and provide sequences of ‘NOW’ moments of conscious experience. Connected to fundamental spacetime geometry by Penrose ‘OR’, consciousness is quantum state reduction, a set of irreversible steps which ‘ratchet forward’ in the fine scale geometry of the universe, creating a flow of time.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-01-04</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>International Journal of Wood Culture</t>
+          <t>Timing &amp; Time Perception</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4210185514</t>
+          <t>https://openalex.org/S4210181418</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -863,17 +863,17 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2772-3186</t>
+          <t>2213-445X</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/27723194-bja10017</t>
+          <t>https://doi.org/10.1163/22134468-bja10098</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>https://brill.com/downloadpdf/journals/ijwc/aop/article-10.1163-27723194-bja10017/article-10.1163-27723194-bja10017.pdf</t>
+          <t>https://brill.com/downloadpdf/view/journals/time/aop/article-10.1163-22134468-bja10098/article-10.1163-22134468-bja10098.pdf</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -888,22 +888,22 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>158</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>167</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="S4" t="b">
@@ -914,16 +914,16 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>diamond</t>
+          <t>hybrid</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>https://brill.com/downloadpdf/journals/ijwc/aop/article-10.1163-27723194-bja10017/article-10.1163-27723194-bja10017.pdf</t>
+          <t>https://brill.com/downloadpdf/view/journals/time/aop/article-10.1163-22134468-bja10098/article-10.1163-22134468-bja10098.pdf</t>
         </is>
       </c>
       <c r="W4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -938,12 +938,12 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4313596414</t>
+          <t>https://api.openalex.org/works?filter=cites:W4388460035</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/27723194-bja10017</t>
+          <t>https://doi.org/10.1163/22134468-bja10098</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
@@ -1192,37 +1192,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4388943180</t>
+          <t>https://openalex.org/W4389207160</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Doctrinal Engagements and Disengagements: Yongming Yanshou and His Legacies</t>
+          <t>Art, Allegory, and the Rise of Shiism in Iran, 1487–1565, written by Chad Kia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Doctrinal Engagements and Disengagements: Yongming Yanshou and His Legacies</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Abstract This paper looks at the vexed relationship of doctrine, or teaching (C. jiao /K. kyo /J. kyō 教 ) in the three kindred traditions subsumed under the rubric of the Sino-East Asian graph 禪 , known through their distinctive pronunciations in modern languages as Chan, Sŏn, and Zen. While the stipulation of these traditions as ‘a special/separate transmission outside the teachings’; (jiaowai biechuan 教外別傳 ) presumes independence from Mahayana doctrinal teachings, the reality, as we know, was much more complicated. In this paper, I use Yongming Yanshou 永明延壽 (904–975/6), one of the most prominent Chan figures to promote doctrinal engagement, as a barometer to look at how doctrinal engagements and disengagements are regarded throughout each tradition. Perspectives on Yanshou, a figure at once revered and marginalized, unlock key features of each of these three interconnected traditions, what they share and how they disagree. Fundamentally, perspectives on doctrinal engagements and disengagements are rooted in seminal Chan disputes over the nature and value of Buddhist teaching, and Yanshou is a conduit for these disputes. Given the theme of the conference, ‘How Zen Became Chan’; I also look at the discrepancies these disputes reveal between modern Rinzai Zen orthodoxy’s defining of Zen in the modern world and the practice of Chan in China and Sŏn in Korea. The options that these discrepancies reveal are indicative of the relevance of doctrinal entanglements and disentanglements to the contemporary Chan, Sŏn, and Zen worlds.</t>
+          <t>Art, Allegory, and the Rise of Shiism in Iran, 1487–1565, written by Chad Kia</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-11-22</t>
+          <t>2023-11-14</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Journal of Chan Buddhism</t>
+          <t>Shii Studies Review</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4210237834</t>
+          <t>https://openalex.org/S4210224839</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1232,27 +1227,27 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2589-7160</t>
+          <t>2468-2462</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/25897179-12340020</t>
+          <t>https://doi.org/10.1163/24682470-12340096</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>409</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>412</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1287,12 +1282,12 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4388943180</t>
+          <t>https://api.openalex.org/works?filter=cites:W4389207160</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/25897179-12340020</t>
+          <t>https://doi.org/10.1163/24682470-12340096</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
@@ -1310,32 +1305,37 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4389207160</t>
+          <t>https://openalex.org/W4388943180</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Art, Allegory, and the Rise of Shiism in Iran, 1487–1565, written by Chad Kia</t>
+          <t>Doctrinal Engagements and Disengagements: Yongming Yanshou and His Legacies</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Art, Allegory, and the Rise of Shiism in Iran, 1487–1565, written by Chad Kia</t>
+          <t>Doctrinal Engagements and Disengagements: Yongming Yanshou and His Legacies</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Abstract This paper looks at the vexed relationship of doctrine, or teaching (C. jiao /K. kyo /J. kyō 教 ) in the three kindred traditions subsumed under the rubric of the Sino-East Asian graph 禪 , known through their distinctive pronunciations in modern languages as Chan, Sŏn, and Zen. While the stipulation of these traditions as ‘a special/separate transmission outside the teachings’; (jiaowai biechuan 教外別傳 ) presumes independence from Mahayana doctrinal teachings, the reality, as we know, was much more complicated. In this paper, I use Yongming Yanshou 永明延壽 (904–975/6), one of the most prominent Chan figures to promote doctrinal engagement, as a barometer to look at how doctrinal engagements and disengagements are regarded throughout each tradition. Perspectives on Yanshou, a figure at once revered and marginalized, unlock key features of each of these three interconnected traditions, what they share and how they disagree. Fundamentally, perspectives on doctrinal engagements and disengagements are rooted in seminal Chan disputes over the nature and value of Buddhist teaching, and Yanshou is a conduit for these disputes. Given the theme of the conference, ‘How Zen Became Chan’; I also look at the discrepancies these disputes reveal between modern Rinzai Zen orthodoxy’s defining of Zen in the modern world and the practice of Chan in China and Sŏn in Korea. The options that these discrepancies reveal are indicative of the relevance of doctrinal entanglements and disentanglements to the contemporary Chan, Sŏn, and Zen worlds.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-11-14</t>
+          <t>2023-11-22</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Shii Studies Review</t>
+          <t>Journal of Chan Buddhism</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4210224839</t>
+          <t>https://openalex.org/S4210237834</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1345,27 +1345,27 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2468-2462</t>
+          <t>2589-7160</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/24682470-12340096</t>
+          <t>https://doi.org/10.1163/25897179-12340020</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>35</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>67</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1400,12 +1400,12 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4389207160</t>
+          <t>https://api.openalex.org/works?filter=cites:W4388943180</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/24682470-12340096</t>
+          <t>https://doi.org/10.1163/25897179-12340020</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">

</xml_diff>